<commit_message>
update JE tblJeu et script insert
pour le problème de course
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc - Copie.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc - Copie.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="633" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="633" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tblMode" sheetId="1" r:id="rId1"/>
@@ -4787,8 +4787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4955,7 +4955,7 @@
         <v>368</v>
       </c>
       <c r="G7">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -4978,7 +4978,7 @@
         <v>368</v>
       </c>
       <c r="G8">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -5001,7 +5001,7 @@
         <v>368</v>
       </c>
       <c r="G9">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -5516,7 +5516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>